<commit_message>
Final Commit. Testing OK
</commit_message>
<xml_diff>
--- a/Historical.xlsx
+++ b/Historical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Part 4 SOFTENG\762\MovieSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB900DE0-FDCC-452A-B43F-8194C2171F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02A1F9A-02B0-44EF-B948-BCBB008118B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2F4EA525-A6D6-4056-8444-ADD700FF158A}"/>
+    <workbookView xWindow="-10590" yWindow="4500" windowWidth="21600" windowHeight="11385" xr2:uid="{2F4EA525-A6D6-4056-8444-ADD700FF158A}"/>
   </bookViews>
   <sheets>
     <sheet name="HistoricalData" sheetId="2" r:id="rId1"/>
@@ -35,22 +35,373 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
+  <si>
+    <t>Collected at:10/17/2021 16:56:55</t>
+  </si>
+  <si>
+    <t>For month:October, 2021</t>
+  </si>
+  <si>
+    <t>Movie Name</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Worldwide</t>
+  </si>
+  <si>
+    <t>Producers</t>
+  </si>
+  <si>
+    <t>Associate Producers</t>
+  </si>
+  <si>
+    <t>Executive Producers</t>
+  </si>
+  <si>
+    <t>Other Producers</t>
+  </si>
+  <si>
+    <t>Directors</t>
+  </si>
+  <si>
+    <t>Venom: Let There Be Carnage</t>
+  </si>
+  <si>
+    <t>Sony Pictures Entertainment (SPE)</t>
+  </si>
+  <si>
+    <t>Avi Arad / Tom Hardy / Kelly Marcel / Hutch Parker / Amy Pascal / Matt Tolmach</t>
+  </si>
+  <si>
+    <t>Jonathan Cavendish / Howard Chen / Edward Cheng / Ruben Fleischer / Barry H. Waldman</t>
+  </si>
+  <si>
+    <t>Barrie Hemsley (co-producer) / Caroline Levy (line producer: additional footage) / Angus More Gordon (co-producer)</t>
+  </si>
+  <si>
+    <t>Andy Serkis</t>
+  </si>
+  <si>
+    <t>No Time to Die</t>
+  </si>
+  <si>
+    <t>Metro-Goldwyn-Mayer (MGM)</t>
+  </si>
+  <si>
+    <t>Barbara Broccoli / Michael G. Wilson</t>
+  </si>
+  <si>
+    <t>Gregg Wilson</t>
+  </si>
+  <si>
+    <t>Chris Brigham</t>
+  </si>
+  <si>
+    <t>Per Henry Borch (line producer: Norway) / Daniel Craig (co-producer) / Andrew Noakes (co-producer) / David Pope (co-producer) / Enzo Sisti (line producer: italy) / Natalie Thompson (line producer: jamaica)</t>
+  </si>
+  <si>
+    <t>Cary Joji Fukunaga</t>
+  </si>
+  <si>
+    <t>The Addams Family 2</t>
+  </si>
+  <si>
+    <t>United Artists Releasing</t>
+  </si>
+  <si>
+    <t>Gail Berman / Alison O'Brien / Danielle Sterling / Conrad Vernon</t>
+  </si>
+  <si>
+    <t>Jason Cloth / Aaron L. Gilbert / Jonathan Glickman / Cassidy Lange / Kevin Miserocchi / Andrew Mittman</t>
+  </si>
+  <si>
+    <t>Barbara Zelinski (line producer)</t>
+  </si>
+  <si>
+    <t>Greg Tiernan / Conrad Vernon / Laura Brousseau / Kevin Pavlovic</t>
+  </si>
+  <si>
+    <t>Halloween Kills</t>
+  </si>
+  <si>
+    <t>Universal Pictures</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>Malek Akkad / Bill Block / Jason Blum</t>
+  </si>
+  <si>
+    <t>Laura Altmann / Scott Clackum</t>
+  </si>
+  <si>
+    <t>John Carpenter / Jamie Lee Curtis / Ryan Freimann / Andrew Golov / David Gordon Green / Danny McBride / Bob Osher / Couper Samuelson / Jeanette Volturno</t>
+  </si>
+  <si>
+    <t>Sean Gowrie (co-producer) / Rick Osako (co-producer (as Rick A. Osako)) / Ryan Turek (co-producer) / Atilla Salih Yücer (co-producer)</t>
+  </si>
+  <si>
+    <t>David Gordon Green</t>
+  </si>
+  <si>
+    <t>The Many Saints of Newark</t>
+  </si>
+  <si>
+    <t>Warner Bros.</t>
+  </si>
+  <si>
+    <t>David Chase / Lawrence Konner / Nicole Lambert</t>
+  </si>
+  <si>
+    <t>Richard Brener / Michael Disco / Toby Emmerich / Marcus Viscidi</t>
+  </si>
+  <si>
+    <t>Alan Taylor</t>
+  </si>
+  <si>
+    <t>The Last Duel</t>
+  </si>
+  <si>
+    <t>Twentieth Century Fox</t>
+  </si>
+  <si>
+    <t>Ben Affleck / Matt Damon / Jennifer Fox / Nicole Holofcener / Ridley Scott / Kevin J. Walsh</t>
+  </si>
+  <si>
+    <t>Sasha Veneziano</t>
+  </si>
+  <si>
+    <t>Madison Ainley / Kevin Halloran / Drew Vinton</t>
+  </si>
+  <si>
+    <t>Aidan Elliott (co-producer) / James Flynn (producer: Metropolitan Films)</t>
+  </si>
+  <si>
+    <t>Ridley Scott</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>Piodor Gustafsson / Hrönn Kristinsdóttir / Sara Nassim / Jan Naszewski / Erik Rydell / Klaudia Smieja</t>
+  </si>
+  <si>
+    <t>Alicja Grawon / Helgi Jóhannsson / Marcin Luczaj</t>
+  </si>
+  <si>
+    <t>Marcin Drabinski / Jon Mankell / Håkan Pettersson / Peter Possne / Noomi Rapace / Béla Tarr</t>
+  </si>
+  <si>
+    <t>Zuzanna Hencz (co-producer)</t>
+  </si>
+  <si>
+    <t>Valdimar Jóhannsson</t>
+  </si>
+  <si>
+    <t>Titane</t>
+  </si>
+  <si>
+    <t>Neon</t>
+  </si>
+  <si>
+    <t>Jean-Christophe Reymond</t>
+  </si>
+  <si>
+    <t>Philippe Logie</t>
+  </si>
+  <si>
+    <t>Christophe Hollebeke</t>
+  </si>
+  <si>
+    <t>Anne-Laure Declerck (assistant producer) / Olivier Père (co-producer) / Jean-Yves Roubin (co-producer) / Cassandre Warnauts (co-producer)</t>
+  </si>
+  <si>
+    <t>Julia Ducournau</t>
+  </si>
+  <si>
+    <t>The Jesus Music</t>
+  </si>
+  <si>
+    <t>Lionsgate</t>
+  </si>
+  <si>
+    <t>Brandon Gregory / Josh Walsh</t>
+  </si>
+  <si>
+    <t>Katelyn Botsch</t>
+  </si>
+  <si>
+    <t>Kevin Downes / Andrew Erwin / Jon Erwin / Amy Grant / Greg Ham / Bill Reeves / Michael W. Smith / Tony Young</t>
+  </si>
+  <si>
+    <t>Parker Adams (co-producer) / Kyle Benn (co-producer) / Ben Field (co-producer) / Bekah Hubbell (Story Producer) / Kristopher Kimlin (co-producer) / Brian Mitchell (co-executive producer) / Ryan Whitaker (Story Producer) / Ben Woods (co-producer)</t>
+  </si>
+  <si>
+    <t>Andrew Erwin / Jon Erwin</t>
+  </si>
+  <si>
+    <t>Chal Mera Putt 3</t>
+  </si>
+  <si>
+    <t>Rhythm Boyz Entertainment</t>
+  </si>
+  <si>
+    <t>Karaj Gill / Munish Sahni</t>
+  </si>
+  <si>
+    <t>Janjot Singh</t>
+  </si>
+  <si>
+    <t>Met Opera: Boris Godunov</t>
+  </si>
+  <si>
+    <t>Fathom Events</t>
+  </si>
+  <si>
+    <t>Old Henry</t>
+  </si>
+  <si>
+    <t>Shout! Factory</t>
+  </si>
+  <si>
+    <t>Michael Hagerty / Shannon Houchins</t>
+  </si>
+  <si>
+    <t>Margaret Miller / Eric Williams</t>
+  </si>
+  <si>
+    <t>Bob Emmer / Jordan Fields / Garson Foos / Richard Foos / Trevor O'Neil / Potsy Ponciroli / Alex Siskin</t>
+  </si>
+  <si>
+    <t>Tamera Brooks (line producer) / Bob Burris (co-producer) / Chris Conner (co-producer) / Jamie R. Thompson (co-producer)</t>
+  </si>
+  <si>
+    <t>Potsy Ponciroli</t>
+  </si>
+  <si>
+    <t>Falling for Figaro</t>
+  </si>
+  <si>
+    <t>IFC Films</t>
+  </si>
+  <si>
+    <t>Judi Levine / Arabella Page Croft / Philip Wade</t>
+  </si>
+  <si>
+    <t>Charles Hannah / Donall McCusker / Kieran Parker / John Wade / Timothy White</t>
+  </si>
+  <si>
+    <t>Ben Lewin</t>
+  </si>
+  <si>
+    <t>Possession</t>
+  </si>
+  <si>
+    <t>Metrograph Pictures</t>
+  </si>
+  <si>
+    <t>Marie-Laure Reyre</t>
+  </si>
+  <si>
+    <t>Andrzej Zulawski</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Bleecker Street Media</t>
+  </si>
+  <si>
+    <t>Fran Kranz / Dylan Matlock / Casey Wilder Mott / J.P. Ouellette</t>
+  </si>
+  <si>
+    <t>Joe Abrams / Nico Falls / Douglas Matejka / Marshall Rawlings</t>
+  </si>
+  <si>
+    <t>Tony Becerra (co-producer) / William Thomas Andrew Davies (co-producer) / J. Davis (consulting producer) / Marissa Ghavami (co-producer)</t>
+  </si>
+  <si>
+    <t>Fran Kranz</t>
+  </si>
+  <si>
+    <t>Golden Voices</t>
+  </si>
+  <si>
+    <t>Music Box Films</t>
+  </si>
+  <si>
+    <t>Leon Edery / Moshe Edery / Eitan Evan / Tami Leon / Chilik Michaeli / Avraham Pirchi</t>
+  </si>
+  <si>
+    <t>Michal Wintroib (line producer)</t>
+  </si>
+  <si>
+    <t>Evgeny Ruman</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>MTV Documentary Films</t>
+  </si>
+  <si>
+    <t>Ronald Gilbert</t>
+  </si>
+  <si>
+    <t>Samantha Ellison / Matt Varosky</t>
+  </si>
+  <si>
+    <t>Jason Blum / Brett Burlock / Tim Gamble / Philip Levens / Mark Stern / Matthew Kaplan</t>
+  </si>
+  <si>
+    <t>Gary Evans (co-producer / associate producer (3 episodes, 2014)) / Ric Nish (co-producer (2 episodes, 2014))</t>
+  </si>
+  <si>
+    <t>Mairzee Almas / Nick Copus / Robert Lieberman / Vincenzo Natali / Stephen Williams</t>
+  </si>
+  <si>
+    <t>Mayday</t>
+  </si>
+  <si>
+    <t>Magnolia Pictures</t>
+  </si>
+  <si>
+    <t>Karen Cinorre / Jonah Disend / Lucas Joaquin / Sam Levy</t>
+  </si>
+  <si>
+    <t>Gabriella Ludlow</t>
+  </si>
+  <si>
+    <t>Jure Busic (line producer) / Amanda Messenger (co-producer)</t>
+  </si>
+  <si>
+    <t>Karen Cinorre</t>
+  </si>
+  <si>
+    <t>Collected at:10/17/2021 16:56:56</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,16 +427,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,28 +747,583 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89490DA4-C70F-495D-AD5B-A9D9A9DDE9B6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="5" width="17.85546875" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
+        <v>156157670</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43900000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>200057670</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>82418249</v>
+      </c>
+      <c r="D4" s="1">
+        <v>259028000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>341446249</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36970524</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5926000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42896524</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>22800000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1">
+        <v>22800000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7938103</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2910205</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10848308</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1863000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1863000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1666861</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1696</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1668557</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1207488</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2789720</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3997208</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1">
+        <v>953470</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1">
+        <v>953470</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1">
+        <v>644000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1377248</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2021248</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="1">
+        <v>387000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>187167</v>
+      </c>
+      <c r="E13" s="1">
+        <v>574167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="1">
+        <v>37194</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1">
+        <v>37194</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="1">
+        <v>30803</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1">
+        <v>30803</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24232</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1">
+        <v>24232</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1">
+        <v>21429</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1">
+        <v>21429</v>
+      </c>
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1">
+        <v>9905</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18407</v>
+      </c>
+      <c r="E18" s="1">
+        <v>28312</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8365</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1">
+        <v>8365</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4382</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4382</v>
+      </c>
+      <c r="F20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2170C21-28ED-43AE-9245-AA08E8EF63F8}">
-  <dimension ref="C1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +1333,279 @@
     <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>341446249</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>200057670</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42896524</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1">
+        <v>22800000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10848308</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3997208</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2021248</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1863000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1668557</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1">
+        <v>953470</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1">
+        <v>574167</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="1">
+        <v>37194</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="1">
+        <v>30803</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1">
+        <v>28312</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1">
+        <v>24232</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="1">
+        <v>21429</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8365</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4382</v>
+      </c>
+      <c r="D20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>